<commit_message>
beginning of results section
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-master.xlsx
+++ b/data/metapopulation-inputs-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74F8EE4-8335-0A4C-9F44-8516323A0E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEAB968-7218-6F4D-A7A4-D91D67078096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
@@ -65,6 +65,7 @@
     <author>tc={0A493894-0BE2-3646-9CA8-F6EB43E39E12}</author>
     <author>tc={E3294B68-B3C5-4A43-B614-3E4CB6542780}</author>
     <author>tc={3844B481-F1F1-B448-A37D-14DB0AD39FFD}</author>
+    <author>tc={64CC0157-61C7-0C4E-9796-EB847F5CFAAE}</author>
     <author>tc={D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}</author>
   </authors>
   <commentList>
@@ -135,7 +136,15 @@
     This is the prevalence at which the IFR is at the midpoint between normal and a worst-case scenario</t>
       </text>
     </comment>
-    <comment ref="D22" authorId="8" shapeId="0" xr:uid="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
+    <comment ref="D21" authorId="8" shapeId="0" xr:uid="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Originally, 0.15</t>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="9" shapeId="0" xr:uid="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -995,6 +1004,9 @@
   <threadedComment ref="D19" dT="2023-07-31T15:00:08.56" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{3844B481-F1F1-B448-A37D-14DB0AD39FFD}">
     <text>This is the prevalence at which the IFR is at the midpoint between normal and a worst-case scenario</text>
   </threadedComment>
+  <threadedComment ref="D21" dT="2024-02-21T15:14:55.07" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
+    <text>Originally, 0.15</text>
+  </threadedComment>
   <threadedComment ref="D22" dT="2024-01-26T19:42:11.64" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
     <text>Was 7</text>
   </threadedComment>
@@ -1059,7 +1071,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1429,7 +1441,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="7">
-        <v>0.15</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
@@ -1446,7 +1458,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="18">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
sensitivity analysis results with epi and societal inputs are sensible
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-master.xlsx
+++ b/data/metapopulation-inputs-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEAB968-7218-6F4D-A7A4-D91D67078096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386DA4D9-BA9D-3648-A702-629D991239F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
@@ -21,18 +21,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parameters!$A$1:$E$35</definedName>
-    <definedName name="c_">parameters!#REF!</definedName>
-    <definedName name="C_surv">parameters!$D$8</definedName>
-    <definedName name="days_to_adjust_NPI">parameters!#REF!</definedName>
-    <definedName name="delta">parameters!$D$3</definedName>
-    <definedName name="gamma">parameters!$D$4</definedName>
-    <definedName name="o">parameters!#REF!</definedName>
-    <definedName name="obs_lag">parameters!$D$7</definedName>
-    <definedName name="r_">parameters!#REF!</definedName>
-    <definedName name="sigma">parameters!$D$2</definedName>
-    <definedName name="tau">parameters!$D$6</definedName>
-    <definedName name="VSLY">parameters!$D$22</definedName>
-    <definedName name="w">parameters!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,6 +50,7 @@
     <author>tc={02ECA6D2-2F52-1849-B877-B94D683D822E}</author>
     <author>tc={D589F124-8EBC-C041-A7B4-6EC8817C3759}</author>
     <author>tc={8B0BC900-2421-E049-9E6B-4777CBF6BEE4}</author>
+    <author>tc={5B19C8E6-302A-2C4E-AD17-FFF89DD9C276}</author>
     <author>tc={0A493894-0BE2-3646-9CA8-F6EB43E39E12}</author>
     <author>tc={E3294B68-B3C5-4A43-B614-3E4CB6542780}</author>
     <author>tc={3844B481-F1F1-B448-A37D-14DB0AD39FFD}</author>
@@ -109,7 +98,15 @@
     Was 1/9</t>
       </text>
     </comment>
-    <comment ref="E8" authorId="5" shapeId="0" xr:uid="{0A493894-0BE2-3646-9CA8-F6EB43E39E12}">
+    <comment ref="D6" authorId="5" shapeId="0" xr:uid="{5B19C8E6-302A-2C4E-AD17-FFF89DD9C276}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Age-adjusted = 0.733%</t>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="6" shapeId="0" xr:uid="{0A493894-0BE2-3646-9CA8-F6EB43E39E12}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -118,7 +115,7 @@
 https://www.ncbi.nlm.nih.gov/pmc/articles/PMC7499700/</t>
       </text>
     </comment>
-    <comment ref="D18" authorId="6" shapeId="0" xr:uid="{E3294B68-B3C5-4A43-B614-3E4CB6542780}">
+    <comment ref="D18" authorId="7" shapeId="0" xr:uid="{E3294B68-B3C5-4A43-B614-3E4CB6542780}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -128,7 +125,7 @@
     This is the maximum prevalence the hospital system can possibly take.</t>
       </text>
     </comment>
-    <comment ref="D19" authorId="7" shapeId="0" xr:uid="{3844B481-F1F1-B448-A37D-14DB0AD39FFD}">
+    <comment ref="D19" authorId="8" shapeId="0" xr:uid="{3844B481-F1F1-B448-A37D-14DB0AD39FFD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -136,15 +133,17 @@
     This is the prevalence at which the IFR is at the midpoint between normal and a worst-case scenario</t>
       </text>
     </comment>
-    <comment ref="D21" authorId="8" shapeId="0" xr:uid="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
+    <comment ref="D21" authorId="9" shapeId="0" xr:uid="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Originally, 0.15</t>
+    Originally, 0.15
+Reply:
+    Calibrated with 1.5 variant strain at 0.137</t>
       </text>
     </comment>
-    <comment ref="D22" authorId="9" shapeId="0" xr:uid="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
+    <comment ref="D22" authorId="10" shapeId="0" xr:uid="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -985,6 +984,9 @@
   <threadedComment ref="D5" dT="2024-01-26T21:27:55.79" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{8B0BC900-2421-E049-9E6B-4777CBF6BEE4}">
     <text>Was 1/9</text>
   </threadedComment>
+  <threadedComment ref="D6" dT="2024-02-23T22:32:02.93" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{5B19C8E6-302A-2C4E-AD17-FFF89DD9C276}">
+    <text>Age-adjusted = 0.733%</text>
+  </threadedComment>
   <threadedComment ref="E8" dT="2023-10-12T12:09:36.52" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{0A493894-0BE2-3646-9CA8-F6EB43E39E12}">
     <text>This paper clarifies the difference between Willingess to pay to avoid risk and willingness to accept new risk, and argues that WTA is more appropriate:
 https://www.ncbi.nlm.nih.gov/pmc/articles/PMC7499700/</text>
@@ -1006,6 +1008,9 @@
   </threadedComment>
   <threadedComment ref="D21" dT="2024-02-21T15:14:55.07" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
     <text>Originally, 0.15</text>
+  </threadedComment>
+  <threadedComment ref="D21" dT="2024-02-23T22:29:25.05" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{DC124B1D-D0F3-994F-B467-F0CAA81F27EA}" parentId="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
+    <text>Calibrated with 1.5 variant strain at 0.137</text>
   </threadedComment>
   <threadedComment ref="D22" dT="2024-01-26T19:42:11.64" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
     <text>Was 7</text>
@@ -1068,10 +1073,10 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1182,7 +1187,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="5">
-        <v>7.3299999999999997E-3</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -1595,7 +1600,7 @@
         <v>104</v>
       </c>
       <c r="D30" s="7">
-        <f>ROUND(1/sigma+1/delta+D29,0)</f>
+        <f>ROUND(1/D2+1/D3+D29,0)</f>
         <v>13</v>
       </c>
       <c r="E30" t="s">
@@ -1717,7 +1722,7 @@
         <v>109</v>
       </c>
       <c r="D37" s="10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
         <v>110</v>
@@ -1734,7 +1739,7 @@
         <v>111</v>
       </c>
       <c r="D38">
-        <v>180</v>
+        <v>1000</v>
       </c>
       <c r="E38" t="s">
         <v>112</v>
@@ -1751,7 +1756,7 @@
         <v>113</v>
       </c>
       <c r="D39">
-        <v>240</v>
+        <v>1001</v>
       </c>
       <c r="E39" t="s">
         <v>114</v>
@@ -1900,7 +1905,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
cleaning up run_analysis script
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-master.xlsx
+++ b/data/metapopulation-inputs-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF80D4C-955C-3146-9D01-457E28CA2400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C324EF0-FEC4-224F-8EEF-F7110BCB4888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="18160" yWindow="-20760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
     </comment>
     <comment ref="D21" authorId="9" shapeId="0" xr:uid="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Originally, 0.15
@@ -148,12 +148,14 @@
     Calibrated with age-adjusted IFR:
 solution$par
          c        tau 
-12.5096989  0.1188833 </t>
+12.5096989  0.1188833 
+Reply:
+    Calibrated again with deaths target of 144.45 (mean deaths per 100k people across US states) and 112 days of maximum intervention level (median computed across US states).</t>
       </text>
     </comment>
     <comment ref="D22" authorId="10" shapeId="0" xr:uid="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Was 7
@@ -165,7 +167,9 @@
     Calibrated with age-adjusted IFR:
 solution$par
          c        tau 
-12.5096989  0.1188833 </t>
+12.5096989  0.1188833 
+Reply:
+    Calibrated again with deaths target of 144.45 (mean deaths per 100k people across US states) and 112 days of maximum intervention level (median computed across US states).</t>
       </text>
     </comment>
   </commentList>
@@ -1037,6 +1041,9 @@
     <text xml:space="preserve">Calibrated with age-adjusted IFR:
 solution$par_x000D_         c        tau _x000D_12.5096989  0.1188833 </text>
   </threadedComment>
+  <threadedComment ref="D21" dT="2024-02-28T22:21:47.30" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{7D931A60-9BD7-7645-AD0D-0A1A6D0128E4}" parentId="{64CC0157-61C7-0C4E-9796-EB847F5CFAAE}">
+    <text>Calibrated again with deaths target of 144.45 (mean deaths per 100k people across US states) and 112 days of maximum intervention level (median computed across US states).</text>
+  </threadedComment>
   <threadedComment ref="D22" dT="2024-01-26T19:42:11.64" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
     <text>Was 7</text>
   </threadedComment>
@@ -1051,6 +1058,9 @@
 solution$par
          c        tau 
 12.5096989  0.1188833 </text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2024-02-28T22:22:06.98" personId="{3AABDFAA-7D8C-674E-BCF6-F68A3F52C914}" id="{C8BEA2BE-7C4A-3046-85A9-7244E96076D1}" parentId="{D8CCF875-0E4B-7C40-BA99-EEFE3C00154E}">
+    <text>Calibrated again with deaths target of 144.45 (mean deaths per 100k people across US states) and 112 days of maximum intervention level (median computed across US states).</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1483,7 +1493,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="10">
-        <v>0.1188833</v>
+        <v>0.1422919</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
@@ -1500,7 +1510,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="18">
-        <v>12.5096989</v>
+        <v>17.913607599999999</v>
       </c>
       <c r="E22" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
updating results with recent parameters and recent calibration
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-master.xlsx
+++ b/data/metapopulation-inputs-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C324EF0-FEC4-224F-8EEF-F7110BCB4888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35C3753-E01E-CF42-A5AF-2FF620F0DFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18160" yWindow="-20760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -602,36 +602,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -648,26 +624,23 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1120,10 +1093,10 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1118,7 @@
       <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1162,7 +1135,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <f>1/3.3</f>
         <v>0.30303030303030304</v>
       </c>
@@ -1180,7 +1153,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <f>1/3.5</f>
         <v>0.2857142857142857</v>
       </c>
@@ -1198,7 +1171,7 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
@@ -1216,7 +1189,7 @@
       <c r="C5" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>0.35</v>
       </c>
       <c r="E5" t="s">
@@ -1233,7 +1206,7 @@
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>7.3299999999999997E-3</v>
       </c>
       <c r="E6" t="s">
@@ -1250,7 +1223,7 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>2.5</v>
       </c>
       <c r="E7" t="s">
@@ -1267,7 +1240,7 @@
       <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="8">
         <v>279113</v>
       </c>
       <c r="E8" t="s">
@@ -1285,9 +1258,9 @@
       <c r="C9" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="15">
-        <f>11.4*10^6</f>
-        <v>11400000</v>
+      <c r="D9" s="9">
+        <f>10.6*10^6</f>
+        <v>10600000</v>
       </c>
       <c r="E9" t="s">
         <v>95</v>
@@ -1303,7 +1276,7 @@
       <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="10">
         <v>0.25</v>
       </c>
       <c r="E10" t="s">
@@ -1320,7 +1293,7 @@
       <c r="C11" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>76000</v>
       </c>
       <c r="E11" t="s">
@@ -1337,7 +1310,7 @@
       <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="5">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -1405,7 +1378,7 @@
       <c r="C16" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="12">
         <v>0.02</v>
       </c>
       <c r="E16" t="s">
@@ -1422,7 +1395,7 @@
       <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="13">
         <v>0</v>
       </c>
       <c r="E17" t="s">
@@ -1439,7 +1412,7 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="14">
         <f>0.7*2.38/1000/D16</f>
         <v>8.3299999999999999E-2</v>
       </c>
@@ -1457,7 +1430,7 @@
       <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="14">
         <f>D18*0.9</f>
         <v>7.4969999999999995E-2</v>
       </c>
@@ -1475,7 +1448,7 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="7">
         <v>1.5</v>
       </c>
       <c r="E20" t="s">
@@ -1492,7 +1465,7 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="5">
         <v>0.1422919</v>
       </c>
       <c r="E21" t="s">
@@ -1509,7 +1482,7 @@
       <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="15">
         <v>17.913607599999999</v>
       </c>
       <c r="E22" t="s">
@@ -1664,7 +1637,7 @@
       <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="8">
         <v>0</v>
       </c>
       <c r="E31" t="s">
@@ -1715,7 +1688,7 @@
       <c r="C34" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="5">
         <v>0.184</v>
       </c>
       <c r="E34" t="s">
@@ -1732,7 +1705,7 @@
       <c r="C35" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="5">
         <f>0.328+0.09+0.042</f>
         <v>0.46</v>
       </c>
@@ -1750,7 +1723,7 @@
       <c r="C36" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="5">
         <f>1-SUM(D34:D35)</f>
         <v>0.35599999999999998</v>
       </c>
@@ -1768,7 +1741,7 @@
       <c r="C37" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="5">
         <v>1</v>
       </c>
       <c r="E37" t="s">
@@ -1785,7 +1758,7 @@
       <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="7">
         <v>1000</v>
       </c>
       <c r="E38" t="s">
@@ -1802,7 +1775,7 @@
       <c r="C39" t="s">
         <v>113</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="7">
         <v>1001</v>
       </c>
       <c r="E39" t="s">

</xml_diff>

<commit_message>
cleaning up script to run full analysis, both R and bash versions work
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-master.xlsx
+++ b/data/metapopulation-inputs-master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DCCEB2-BB40-E14E-967B-5236EBA2BFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CCC4CB-C677-E340-BA02-2E4AD8552526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="2" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1089,11 +1089,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930774C7-2D37-094A-A2DB-7EC2D5ACBFA8}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1794,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4AC197-751B-D642-B32A-DB1D08A8DC07}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update figures to pdf
</commit_message>
<xml_diff>
--- a/data/metapopulation-inputs-master.xlsx
+++ b/data/metapopulation-inputs-master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/plima/dev/genomic-surveillance-voi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B4498-E426-854C-9710-E1772DC8A165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F610FA6-22E9-CC4A-8744-2E2FF830435C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" activeTab="1" xr2:uid="{0C369B58-09D0-0147-9E6F-D031731E4386}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1093,7 +1093,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>